<commit_message>
add 2 validation bug end with semi colon
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test18_Validation/ExcelQuery.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test18_Validation/ExcelQuery.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="175">
   <si>
     <t>Index</t>
   </si>
@@ -529,6 +529,21 @@
   </si>
   <si>
     <t>Select BOOLEAN pattern s.stmt# = 1</t>
+  </si>
+  <si>
+    <t>Select s such that Follows(1,2);</t>
+  </si>
+  <si>
+    <t>stmt s</t>
+  </si>
+  <si>
+    <t>Selection before Declaration</t>
+  </si>
+  <si>
+    <t>Select boolean in declaration no semi-colon</t>
+  </si>
+  <si>
+    <t>Select boolean in declaration have semi-colon</t>
   </si>
 </sst>
 </file>
@@ -958,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3F969A-AF06-4B88-BDEC-BD9AE21F1F8A}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,58 +1122,63 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="B11" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="7"/>
       <c r="D11" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>18</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C12" s="7" t="s">
-        <v>38</v>
+        <v>167</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>41</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1166,64 +1186,55 @@
         <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="C15" s="7" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="C16" s="7" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1231,16 +1242,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1248,16 +1259,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,7 +1276,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>7</v>
@@ -1274,7 +1285,7 @@
         <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1282,16 +1293,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1299,16 +1310,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1316,16 +1327,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1333,7 +1344,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>7</v>
@@ -1342,7 +1353,7 @@
         <v>8</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1350,16 +1361,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1367,16 +1378,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1384,16 +1395,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1401,16 +1412,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>139</v>
+        <v>7</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1418,16 +1429,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1438,13 +1449,13 @@
         <v>11</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1452,16 +1463,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1469,16 +1480,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1486,16 +1497,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1503,16 +1514,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>139</v>
+        <v>51</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1520,16 +1531,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>139</v>
+        <v>52</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1537,16 +1548,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>140</v>
+        <v>53</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1554,16 +1565,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1571,16 +1582,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>8</v>
+        <v>58</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1588,16 +1599,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>13</v>
+        <v>61</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1605,16 +1616,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>13</v>
+        <v>74</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1622,16 +1633,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1639,16 +1650,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1656,16 +1667,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1673,16 +1684,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1690,16 +1701,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>121</v>
+        <v>20</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>142</v>
+        <v>8</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>151</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1707,16 +1718,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>152</v>
+        <v>20</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1724,16 +1735,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>161</v>
+        <v>8</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1744,13 +1755,13 @@
         <v>121</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1758,16 +1769,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1775,16 +1786,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1792,16 +1803,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>94</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1809,16 +1820,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1826,16 +1837,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>101</v>
+        <v>159</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1846,13 +1857,13 @@
         <v>92</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>13</v>
+        <v>93</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1860,16 +1871,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>13</v>
+        <v>95</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1877,16 +1888,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1894,16 +1905,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1911,16 +1922,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1928,16 +1939,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1945,16 +1956,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1962,10 +1973,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>13</v>
@@ -1979,10 +1990,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>169</v>
+        <v>118</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>13</v>
@@ -1996,10 +2007,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>13</v>
@@ -2013,16 +2024,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2030,16 +2041,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>145</v>
+        <v>169</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2047,16 +2058,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>145</v>
+        <v>129</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2064,16 +2075,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2084,13 +2095,13 @@
         <v>100</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>36</v>
+        <v>105</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2098,16 +2109,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2115,16 +2126,16 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>146</v>
+        <v>109</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2132,16 +2143,16 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2152,13 +2163,13 @@
         <v>124</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>36</v>
+        <v>125</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2166,16 +2177,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>8</v>
+        <v>128</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2183,16 +2194,16 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2200,16 +2211,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2220,7 +2231,7 @@
         <v>134</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>8</v>
@@ -2229,8 +2240,59 @@
         <v>135</v>
       </c>
     </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>75</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>76</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>77</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G76:G1048576 G1:G74">
+  <conditionalFormatting sqref="G79:G1048576 G1:G77">
     <cfRule type="cellIs" dxfId="3" priority="15" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
@@ -2238,7 +2300,7 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G75">
+  <conditionalFormatting sqref="G78">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>

</xml_diff>